<commit_message>
Added BoP capex, opex and deleted old Athens UC folder
</commit_message>
<xml_diff>
--- a/models/Athens DESFA exit point new obj/Data/parameters_guide_new_obj.xlsx
+++ b/models/Athens DESFA exit point new obj/Data/parameters_guide_new_obj.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://epuntuagr-my.sharepoint.com/personal/hkoutalidis_epu_ntua_gr/Documents/Enershare/Paper 2 H2 scenarios paper/P2G_Hydrogen_Repository_remote/models/Athens DESFA exit point new obj/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="225" documentId="11_F25DC773A252ABDACC104899015D5D385ADE58F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6EDC0B0-5D51-42FD-B1DD-B79151FEBB16}"/>
+  <xr:revisionPtr revIDLastSave="256" documentId="11_F25DC773A252ABDACC104899015D5D385ADE58F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CDF4EBC0-54EF-44B6-80E6-B0722EEFB4FB}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Simulations S2.1 (own RES inve)" sheetId="1" r:id="rId1"/>
@@ -329,7 +329,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -358,9 +358,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -666,8 +663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -756,8 +753,8 @@
         <v>24660</v>
       </c>
       <c r="E5" s="7">
-        <f t="shared" si="2"/>
-        <v>21920</v>
+        <f>B5*0.75</f>
+        <v>20550</v>
       </c>
       <c r="F5" s="7"/>
     </row>
@@ -785,7 +782,7 @@
         <v>612000</v>
       </c>
       <c r="E7" s="7">
-        <f t="shared" si="2"/>
+        <f>B7*0.8</f>
         <v>544000</v>
       </c>
       <c r="F7" s="7"/>
@@ -823,12 +820,12 @@
         <v>14487.5</v>
       </c>
       <c r="D9" s="7">
-        <f t="shared" si="1"/>
+        <f>B9*0.9</f>
         <v>13725</v>
       </c>
       <c r="E9" s="7">
-        <f t="shared" si="2"/>
-        <v>12200</v>
+        <f>B9*0.75</f>
+        <v>11437.5</v>
       </c>
       <c r="F9" s="7"/>
     </row>
@@ -992,8 +989,8 @@
         <v>831600</v>
       </c>
       <c r="E21" s="7">
-        <f>D21*0.8</f>
-        <v>665280</v>
+        <f>B21*0.65</f>
+        <v>600600</v>
       </c>
       <c r="F21" s="7"/>
     </row>
@@ -1009,12 +1006,12 @@
         <v>17556</v>
       </c>
       <c r="D22" s="7">
-        <f t="shared" ref="D22" si="3">B22*0.9</f>
+        <f>B22*0.9</f>
         <v>16632</v>
       </c>
       <c r="E22" s="7">
-        <f t="shared" ref="E22" si="4">D22*0.8</f>
-        <v>13305.6</v>
+        <f>B22*0.65</f>
+        <v>12012</v>
       </c>
       <c r="F22" s="7"/>
     </row>
@@ -1129,8 +1126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF26B971-9089-40B6-B7D9-B4FE2F3EF079}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1194,8 +1191,8 @@
         <v>47.7</v>
       </c>
       <c r="E4" s="7">
-        <f>B4*0.8</f>
-        <v>42.400000000000006</v>
+        <f>B4*0.75</f>
+        <v>39.75</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1255,8 +1252,8 @@
         <v>28.62</v>
       </c>
       <c r="E8" s="7">
-        <f>B8*0.8</f>
-        <v>25.44</v>
+        <f>B8*0.75</f>
+        <v>23.85</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1425,8 +1422,8 @@
         <v>831600</v>
       </c>
       <c r="E21" s="7">
-        <f>D21*0.8</f>
-        <v>665280</v>
+        <f>B21*0.65</f>
+        <v>600600</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1445,8 +1442,8 @@
         <v>16632</v>
       </c>
       <c r="E22" s="7">
-        <f t="shared" ref="E22" si="1">D22*0.8</f>
-        <v>13305.6</v>
+        <f>B22*0.65</f>
+        <v>12012</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1462,8 +1459,8 @@
       <c r="D23" s="7">
         <v>1.33</v>
       </c>
-      <c r="E23" s="14">
-        <v>1.06</v>
+      <c r="E23" s="7">
+        <v>1.33</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1544,256 +1541,256 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="16" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" style="16" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" style="16" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" style="16" customWidth="1"/>
-    <col min="6" max="10" width="9.140625" style="16"/>
-    <col min="11" max="11" width="33.5703125" style="16" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" style="16" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" style="16" customWidth="1"/>
-    <col min="14" max="15" width="13.85546875" style="16" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="16"/>
+    <col min="1" max="1" width="29.28515625" style="15" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="15" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" style="15" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" style="15" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="15" customWidth="1"/>
+    <col min="6" max="10" width="9.140625" style="15"/>
+    <col min="11" max="11" width="33.5703125" style="15" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" style="15" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" style="15" customWidth="1"/>
+    <col min="14" max="15" width="13.85546875" style="15" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="K1" s="20" t="s">
+      <c r="K1" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="M1" s="14" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="21" t="s">
+      <c r="K2" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="L2" s="19" t="s">
+      <c r="L2" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="M2" s="19" t="s">
+      <c r="M2" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="N2" s="19" t="s">
+      <c r="N2" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="O2" s="19" t="s">
+      <c r="O2" s="18" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="22">
+      <c r="A3" s="21">
         <v>3</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="17" t="s">
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="K3" s="22">
+      <c r="K3" s="21">
         <v>3.5</v>
       </c>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="18"/>
-      <c r="O3" s="17" t="s">
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="16" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="22">
+      <c r="A4" s="21">
         <v>3.5</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="17" t="s">
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="K4" s="22">
+      <c r="K4" s="21">
         <v>4</v>
       </c>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
-      <c r="N4" s="17" t="s">
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="O4" s="17" t="s">
+      <c r="O4" s="16" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="22">
+      <c r="A5" s="21">
         <v>4</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="K5" s="22">
+      <c r="K5" s="21">
         <v>4.5</v>
       </c>
-      <c r="L5" s="17" t="s">
+      <c r="L5" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="M5" s="17" t="s">
+      <c r="M5" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="N5" s="17" t="s">
+      <c r="N5" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="O5" s="17" t="s">
+      <c r="O5" s="16" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" s="22">
+      <c r="A6" s="21">
         <v>4.5</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="K6" s="22">
+      <c r="K6" s="21">
         <v>5</v>
       </c>
-      <c r="L6" s="17" t="s">
+      <c r="L6" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="M6" s="17" t="s">
+      <c r="M6" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="N6" s="17" t="s">
+      <c r="N6" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="O6" s="17" t="s">
+      <c r="O6" s="16" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="22">
+      <c r="A7" s="21">
         <v>5</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="K7" s="22">
+      <c r="K7" s="21">
         <v>5.5</v>
       </c>
-      <c r="L7" s="17" t="s">
+      <c r="L7" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="M7" s="17" t="s">
+      <c r="M7" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="N7" s="17" t="s">
+      <c r="N7" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="O7" s="17" t="s">
+      <c r="O7" s="16" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="22">
+      <c r="A8" s="21">
         <v>5.5</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="18"/>
-      <c r="K8" s="22">
+      <c r="E8" s="17"/>
+      <c r="K8" s="21">
         <v>6</v>
       </c>
-      <c r="L8" s="17" t="s">
+      <c r="L8" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="M8" s="17" t="s">
+      <c r="M8" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="N8" s="17" t="s">
+      <c r="N8" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="O8" s="18"/>
+      <c r="O8" s="17"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="22">
+      <c r="A9" s="21">
         <v>6</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="K9" s="22">
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="K9" s="21">
         <v>6.5</v>
       </c>
-      <c r="L9" s="17" t="s">
+      <c r="L9" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="M9" s="17" t="s">
+      <c r="M9" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="N9" s="18"/>
-      <c r="O9" s="18"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Input parameters will now be set inside the scripts, instead of read from csv.
</commit_message>
<xml_diff>
--- a/models/Athens DESFA exit point new obj/Data/parameters_guide_new_obj.xlsx
+++ b/models/Athens DESFA exit point new obj/Data/parameters_guide_new_obj.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://epuntuagr-my.sharepoint.com/personal/hkoutalidis_epu_ntua_gr/Documents/Enershare/Paper 2 H2 scenarios paper/P2G_Hydrogen_Repository_remote/models/Athens DESFA exit point new obj/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="256" documentId="11_F25DC773A252ABDACC104899015D5D385ADE58F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CDF4EBC0-54EF-44B6-80E6-B0722EEFB4FB}"/>
+  <xr:revisionPtr revIDLastSave="271" documentId="11_F25DC773A252ABDACC104899015D5D385ADE58F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61D77D15-6CB7-4706-A477-4FA05148193A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Simulations S2.1 (own RES inve)" sheetId="1" r:id="rId1"/>
@@ -38,29 +38,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="35">
   <si>
     <t>Generators</t>
   </si>
   <si>
-    <t>WF capital costs (EUR/MW)</t>
-  </si>
-  <si>
-    <t>WF marginal costs (EUR/MWh)</t>
-  </si>
-  <si>
-    <t>WF Fixed opex  (EUR/MW/year)</t>
-  </si>
-  <si>
-    <t>SF capital costs (EUR/MW)</t>
-  </si>
-  <si>
-    <t>SF marginal costs (EUR/MWh)</t>
-  </si>
-  <si>
-    <t>SF Fixed opex  (EUR/MW/year)</t>
-  </si>
-  <si>
     <t>Electrolyzer</t>
   </si>
   <si>
@@ -76,48 +58,18 @@
     <t>H2 storage</t>
   </si>
   <si>
-    <t>capital cost (EUR/MWh H2)</t>
-  </si>
-  <si>
     <t>Fixed OPEX (EUR/MWh/year)</t>
   </si>
   <si>
     <t>marginal cost (EUR/MWh H2)</t>
   </si>
   <si>
-    <t>charging efficiency</t>
-  </si>
-  <si>
-    <t>discharging efficincy</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>Capexes are scaled for 10 years. If a component has capex C, and lifetime L, then its capex here is C*10/L</t>
-  </si>
-  <si>
-    <t>Fixed OPEX (EUR/MW/year)</t>
-  </si>
-  <si>
     <t>Var Opex (EUR/MWh)</t>
   </si>
   <si>
     <t>Max injection ratio (MHA)</t>
   </si>
   <si>
-    <t>Wind capital costs (EUR/MW)</t>
-  </si>
-  <si>
-    <t>Wind marginal costs (EUR/MWh)</t>
-  </si>
-  <si>
-    <t>Solar capital costs (EUR/MW)</t>
-  </si>
-  <si>
-    <t>Solar marginal costs (EUR/MWh)</t>
-  </si>
-  <si>
     <t xml:space="preserve">sensitivity analysis scenario </t>
   </si>
   <si>
@@ -133,12 +85,6 @@
     <t>LE3</t>
   </si>
   <si>
-    <t>Wind Fixed opex (EUR/MW/year)</t>
-  </si>
-  <si>
-    <t>Solar Fixed opex  (EUR/MW/year)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Max injection ratio (MHA) </t>
   </si>
   <si>
@@ -173,6 +119,30 @@
   </si>
   <si>
     <t xml:space="preserve">Main </t>
+  </si>
+  <si>
+    <t>wind spec capex (EUR/MW)</t>
+  </si>
+  <si>
+    <t>solar spec capex (EUR/MW)</t>
+  </si>
+  <si>
+    <t>wind marginal costs (EUR/MWh)</t>
+  </si>
+  <si>
+    <t>wind Fixed opex  (EUR/MW/year)</t>
+  </si>
+  <si>
+    <t>solar marginal costs (EUR/MWh)</t>
+  </si>
+  <si>
+    <t>solar Fixed opex  (EUR/MW/year)</t>
+  </si>
+  <si>
+    <t>spec capex (EUR/MW)</t>
+  </si>
+  <si>
+    <t>H2 spec capex (EUR/MWh H2)</t>
   </si>
 </sst>
 </file>
@@ -661,10 +631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,16 +648,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -697,7 +667,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="B3" s="7">
         <v>1104000</v>
@@ -718,7 +688,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="B4" s="8">
         <v>0</v>
@@ -728,18 +698,18 @@
         <v>0</v>
       </c>
       <c r="D4" s="8">
-        <f t="shared" ref="D4:D9" si="1">B4*0.9</f>
+        <f t="shared" ref="D4:D8" si="1">B4*0.9</f>
         <v>0</v>
       </c>
       <c r="E4" s="8">
-        <f t="shared" ref="E4:E9" si="2">B4*0.8</f>
+        <f t="shared" ref="E4:E8" si="2">B4*0.8</f>
         <v>0</v>
       </c>
       <c r="F4" s="7"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="B5" s="7">
         <v>27400</v>
@@ -768,7 +738,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="B7" s="7">
         <v>680000</v>
@@ -789,7 +759,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="B8" s="8">
         <v>0</v>
@@ -810,7 +780,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="B9" s="7">
         <v>15250</v>
@@ -845,7 +815,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -855,7 +825,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="B13" s="7">
         <v>14500</v>
@@ -876,7 +846,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B14" s="7">
         <v>290</v>
@@ -897,7 +867,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B15" s="7">
         <v>0</v>
@@ -914,208 +884,155 @@
       <c r="F15" s="7"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="7">
-        <v>0.99</v>
-      </c>
-      <c r="C16" s="7">
-        <v>0.99</v>
-      </c>
-      <c r="D16" s="7">
-        <v>0.99</v>
-      </c>
-      <c r="E16" s="7">
-        <v>0.99</v>
-      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
       <c r="F16" s="7"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="7">
-        <v>0.99</v>
-      </c>
-      <c r="C17" s="7">
-        <v>0.99</v>
-      </c>
-      <c r="D17" s="7">
-        <v>0.99</v>
-      </c>
-      <c r="E17" s="7">
-        <v>0.99</v>
-      </c>
+      <c r="A17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
       <c r="F17" s="7"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
+      <c r="A18" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="7">
+        <v>924000</v>
+      </c>
+      <c r="C18" s="7">
+        <f>B18*0.95</f>
+        <v>877800</v>
+      </c>
+      <c r="D18" s="7">
+        <f>B18*0.9</f>
+        <v>831600</v>
+      </c>
+      <c r="E18" s="7">
+        <f>B18*0.65</f>
+        <v>600600</v>
+      </c>
       <c r="F18" s="7"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
+      <c r="A19" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="7">
+        <v>18480</v>
+      </c>
+      <c r="C19" s="7">
+        <f>B19*0.95</f>
+        <v>17556</v>
+      </c>
+      <c r="D19" s="7">
+        <f>B19*0.9</f>
+        <v>16632</v>
+      </c>
+      <c r="E19" s="7">
+        <f>B19*0.65</f>
+        <v>12012</v>
+      </c>
       <c r="F19" s="7"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
+      <c r="A20" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="7">
+        <v>1.33</v>
+      </c>
+      <c r="C20" s="7">
+        <f>$B$20</f>
+        <v>1.33</v>
+      </c>
+      <c r="D20" s="7">
+        <f>$B$20</f>
+        <v>1.33</v>
+      </c>
+      <c r="E20" s="7">
+        <f>$B$20</f>
+        <v>1.33</v>
+      </c>
       <c r="F20" s="7"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B21" s="7">
-        <v>924000</v>
+        <v>0.75600000000000001</v>
       </c>
       <c r="C21" s="7">
-        <f>B21*0.95</f>
-        <v>877800</v>
-      </c>
-      <c r="D21" s="7">
-        <f>B21*0.9</f>
-        <v>831600</v>
-      </c>
-      <c r="E21" s="7">
-        <f>B21*0.65</f>
-        <v>600600</v>
+        <v>0.79</v>
+      </c>
+      <c r="D21" s="9">
+        <v>0.82</v>
+      </c>
+      <c r="E21" s="9">
+        <v>0.85</v>
       </c>
       <c r="F21" s="7"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="7">
-        <v>18480</v>
-      </c>
-      <c r="C22" s="7">
-        <f>B22*0.95</f>
-        <v>17556</v>
-      </c>
-      <c r="D22" s="7">
-        <f>B22*0.9</f>
-        <v>16632</v>
-      </c>
-      <c r="E22" s="7">
-        <f>B22*0.65</f>
-        <v>12012</v>
-      </c>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
       <c r="F22" s="7"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="7">
-        <v>1.33</v>
-      </c>
-      <c r="C23" s="7">
-        <f>$B$23</f>
-        <v>1.33</v>
-      </c>
-      <c r="D23" s="7">
-        <f>$B$23</f>
-        <v>1.33</v>
-      </c>
-      <c r="E23" s="7">
-        <f>$B$23</f>
-        <v>1.33</v>
+      <c r="A23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="C23" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="D23" s="11">
+        <v>0.3</v>
+      </c>
+      <c r="E23" s="12">
+        <v>0.5</v>
       </c>
       <c r="F23" s="7"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="7">
-        <v>0.75600000000000001</v>
-      </c>
-      <c r="C24" s="7">
-        <v>0.79</v>
-      </c>
-      <c r="D24" s="9">
-        <v>0.82</v>
-      </c>
-      <c r="E24" s="9">
-        <v>0.85</v>
-      </c>
-      <c r="F24" s="7"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
+      <c r="B25" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="F25" s="7"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B26" s="10">
-        <v>0.1</v>
-      </c>
-      <c r="C26" s="10">
-        <v>0.2</v>
-      </c>
-      <c r="D26" s="11">
-        <v>0.3</v>
-      </c>
-      <c r="E26" s="12">
-        <v>0.5</v>
-      </c>
-      <c r="F26" s="7"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F28" s="7"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>1</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>18</v>
-      </c>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1124,10 +1041,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF26B971-9089-40B6-B7D9-B4FE2F3EF079}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1141,16 +1058,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1160,7 +1077,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B3" s="13">
         <v>0</v>
@@ -1177,7 +1094,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B4" s="7">
         <v>53</v>
@@ -1197,7 +1114,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="13">
         <v>0</v>
@@ -1221,7 +1138,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B7" s="13">
         <v>0</v>
@@ -1238,7 +1155,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B8" s="7">
         <v>31.8</v>
@@ -1287,7 +1204,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -1296,7 +1213,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="B13" s="7">
         <v>14500</v>
@@ -1316,7 +1233,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B14" s="7">
         <v>290</v>
@@ -1336,7 +1253,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B15" s="7">
         <v>0</v>
@@ -1352,132 +1269,122 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="7">
-        <v>0.99</v>
-      </c>
-      <c r="C16" s="7">
-        <v>0.99</v>
-      </c>
-      <c r="D16" s="7">
-        <v>0.99</v>
-      </c>
-      <c r="E16" s="7">
-        <v>0.99</v>
-      </c>
+      <c r="A16" s="5"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="7">
-        <v>0.99</v>
-      </c>
-      <c r="C17" s="7">
-        <v>0.99</v>
-      </c>
-      <c r="D17" s="7">
-        <v>0.99</v>
-      </c>
-      <c r="E17" s="7">
-        <v>0.99</v>
-      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
+      <c r="A19" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="7">
+        <v>924000</v>
+      </c>
+      <c r="C19" s="7">
+        <f>B19*0.95</f>
+        <v>877800</v>
+      </c>
+      <c r="D19" s="7">
+        <f>B19*0.9</f>
+        <v>831600</v>
+      </c>
+      <c r="E19" s="7">
+        <f>B19*0.65</f>
+        <v>600600</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
+      <c r="A20" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="7">
+        <v>18480</v>
+      </c>
+      <c r="C20" s="7">
+        <f>B20*0.95</f>
+        <v>17556</v>
+      </c>
+      <c r="D20" s="7">
+        <f t="shared" ref="D20" si="0">B20*0.9</f>
+        <v>16632</v>
+      </c>
+      <c r="E20" s="7">
+        <f>B20*0.65</f>
+        <v>12012</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B21" s="7">
-        <v>924000</v>
+        <v>1.33</v>
       </c>
       <c r="C21" s="7">
-        <f>B21*0.95</f>
-        <v>877800</v>
+        <v>1.33</v>
       </c>
       <c r="D21" s="7">
-        <f>B21*0.9</f>
-        <v>831600</v>
+        <v>1.33</v>
       </c>
       <c r="E21" s="7">
-        <f>B21*0.65</f>
-        <v>600600</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="7">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="C22" s="7">
+        <v>0.79</v>
+      </c>
+      <c r="D22" s="9">
+        <v>0.82</v>
+      </c>
+      <c r="E22" s="9">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="7">
-        <v>18480</v>
-      </c>
-      <c r="C22" s="7">
-        <f>B22*0.95</f>
-        <v>17556</v>
-      </c>
-      <c r="D22" s="7">
-        <f t="shared" ref="D22" si="0">B22*0.9</f>
-        <v>16632</v>
-      </c>
-      <c r="E22" s="7">
-        <f>B22*0.65</f>
-        <v>12012</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="7">
-        <v>1.33</v>
-      </c>
-      <c r="C23" s="7">
-        <v>1.33</v>
-      </c>
-      <c r="D23" s="7">
-        <v>1.33</v>
-      </c>
-      <c r="E23" s="7">
-        <v>1.33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B24" s="7">
-        <v>0.75600000000000001</v>
-      </c>
-      <c r="C24" s="7">
-        <v>0.79</v>
-      </c>
-      <c r="D24" s="9">
-        <v>0.82</v>
-      </c>
-      <c r="E24" s="9">
-        <v>0.85</v>
+      <c r="B24" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="C24" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="D24" s="11">
+        <v>0.3</v>
+      </c>
+      <c r="E24" s="12">
+        <v>0.5</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1487,43 +1394,20 @@
       <c r="E25" s="7"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" s="10">
-        <v>0.1</v>
-      </c>
-      <c r="C26" s="10">
-        <v>0.2</v>
-      </c>
-      <c r="D26" s="11">
-        <v>0.3</v>
-      </c>
-      <c r="E26" s="12">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>30</v>
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1536,7 +1420,7 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1556,48 +1440,48 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="K1" s="19" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="M1" s="14" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="22" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="K2" s="20" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="L2" s="18" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="M2" s="18" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="N2" s="18" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
@@ -1608,7 +1492,7 @@
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
       <c r="E3" s="16" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="K3" s="21">
         <v>3.5</v>
@@ -1617,7 +1501,7 @@
       <c r="M3" s="17"/>
       <c r="N3" s="17"/>
       <c r="O3" s="16" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -1627,10 +1511,10 @@
       <c r="B4" s="17"/>
       <c r="C4" s="17"/>
       <c r="D4" s="16" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="K4" s="21">
         <v>4</v>
@@ -1638,10 +1522,10 @@
       <c r="L4" s="17"/>
       <c r="M4" s="17"/>
       <c r="N4" s="16" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="O4" s="16" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -1649,31 +1533,31 @@
         <v>4</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="K5" s="21">
         <v>4.5</v>
       </c>
       <c r="L5" s="16" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="M5" s="16" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="N5" s="16" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="O5" s="16" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
@@ -1681,31 +1565,31 @@
         <v>4.5</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="K6" s="21">
         <v>5</v>
       </c>
       <c r="L6" s="16" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="M6" s="16" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="N6" s="16" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="O6" s="16" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
@@ -1713,31 +1597,31 @@
         <v>5</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="K7" s="21">
         <v>5.5</v>
       </c>
       <c r="L7" s="16" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="M7" s="16" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="N7" s="16" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="O7" s="16" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
@@ -1745,26 +1629,26 @@
         <v>5.5</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="E8" s="17"/>
       <c r="K8" s="21">
         <v>6</v>
       </c>
       <c r="L8" s="16" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="M8" s="16" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="N8" s="16" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="O8" s="17"/>
     </row>
@@ -1773,10 +1657,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
@@ -1784,10 +1668,10 @@
         <v>6.5</v>
       </c>
       <c r="L9" s="16" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="M9" s="16" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="N9" s="17"/>
       <c r="O9" s="17"/>

</xml_diff>